<commit_message>
Added Test Cases for New Applicant Registration
</commit_message>
<xml_diff>
--- a/TestData/NewApplicantRegestationDataSheet.xlsx
+++ b/TestData/NewApplicantRegestationDataSheet.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14028" windowHeight="7740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14028" windowHeight="7740" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RegestationSheet" sheetId="1" r:id="rId1"/>
     <sheet name="BasicDetailsSheet" sheetId="2" r:id="rId2"/>
-    <sheet name="OTP Validation" sheetId="3" r:id="rId3"/>
+    <sheet name="NewApplicantRegSheet" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <oleSize ref="A1:N25"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:K25"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="112">
   <si>
     <t>FirstName</t>
   </si>
@@ -172,6 +172,192 @@
   </si>
   <si>
     <t xml:space="preserve">SWETA PANDE </t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>TG</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>Religion</t>
+  </si>
+  <si>
+    <t>Caste</t>
+  </si>
+  <si>
+    <t>AnnualIncome</t>
+  </si>
+  <si>
+    <t>BloodGroup</t>
+  </si>
+  <si>
+    <t>MaritalStatus</t>
+  </si>
+  <si>
+    <t>Disablilities</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>Divorced</t>
+  </si>
+  <si>
+    <t>AB+</t>
+  </si>
+  <si>
+    <t>AB-</t>
+  </si>
+  <si>
+    <t>O+</t>
+  </si>
+  <si>
+    <t>O-</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>A-</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>B-</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Foreign(Others)</t>
+  </si>
+  <si>
+    <t>Other Backward Classes</t>
+  </si>
+  <si>
+    <t>SPORTS QUOTA</t>
+  </si>
+  <si>
+    <t>Minority</t>
+  </si>
+  <si>
+    <t>Foreign(Bangladesh)</t>
+  </si>
+  <si>
+    <t>Hinduism</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>Greek</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Below &lt; 1,00,000</t>
+  </si>
+  <si>
+    <t>1,00,000 to 2,50,000</t>
+  </si>
+  <si>
+    <t>2,50,000 to 5,00,000</t>
+  </si>
+  <si>
+    <t>5,00,000 &gt; more</t>
+  </si>
+  <si>
+    <t>Below &lt; 1,00,001</t>
+  </si>
+  <si>
+    <t>1,00,000 to 2,50,001</t>
+  </si>
+  <si>
+    <t>2,50,000 to 5,00,001</t>
+  </si>
+  <si>
+    <t>Below &lt; 1,00,002</t>
+  </si>
+  <si>
+    <t>TEST ADDRESS</t>
+  </si>
+  <si>
+    <t>PermanentAddressLine1</t>
+  </si>
+  <si>
+    <t>PermanentAddressLine2</t>
+  </si>
+  <si>
+    <t>PermanentCountry</t>
+  </si>
+  <si>
+    <t>PermanentState</t>
+  </si>
+  <si>
+    <t>PermanentDistrict</t>
+  </si>
+  <si>
+    <t>PermanentCity</t>
+  </si>
+  <si>
+    <t>PermanentPin</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>PresentAddressLine1</t>
+  </si>
+  <si>
+    <t>PresentAddressLine2</t>
+  </si>
+  <si>
+    <t>PresentCountry</t>
+  </si>
+  <si>
+    <t>PresentState</t>
+  </si>
+  <si>
+    <t>PresentDistrict</t>
+  </si>
+  <si>
+    <t>PresentCity</t>
+  </si>
+  <si>
+    <t>PresentPin</t>
+  </si>
+  <si>
+    <t>Priya@</t>
+  </si>
+  <si>
+    <t>Desmukh&amp;*</t>
   </si>
 </sst>
 </file>
@@ -502,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -805,12 +991,964 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N1" t="s">
+        <v>95</v>
+      </c>
+      <c r="O1" t="s">
+        <v>96</v>
+      </c>
+      <c r="P1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>98</v>
+      </c>
+      <c r="R1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S1" t="s">
+        <v>103</v>
+      </c>
+      <c r="T1" t="s">
+        <v>104</v>
+      </c>
+      <c r="U1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V1" t="s">
+        <v>106</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+      <c r="X1" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N2" t="s">
+        <v>100</v>
+      </c>
+      <c r="O2" t="s">
+        <v>101</v>
+      </c>
+      <c r="P2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>102</v>
+      </c>
+      <c r="R2">
+        <v>756115</v>
+      </c>
+      <c r="S2" t="s">
+        <v>92</v>
+      </c>
+      <c r="T2" t="s">
+        <v>92</v>
+      </c>
+      <c r="U2" t="s">
+        <v>100</v>
+      </c>
+      <c r="V2" t="s">
+        <v>101</v>
+      </c>
+      <c r="W2" t="s">
+        <v>102</v>
+      </c>
+      <c r="X2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y2">
+        <v>756115</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M3" t="s">
+        <v>92</v>
+      </c>
+      <c r="N3" t="s">
+        <v>100</v>
+      </c>
+      <c r="O3" t="s">
+        <v>101</v>
+      </c>
+      <c r="P3" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>102</v>
+      </c>
+      <c r="R3">
+        <v>756115</v>
+      </c>
+      <c r="S3" t="s">
+        <v>92</v>
+      </c>
+      <c r="T3" t="s">
+        <v>92</v>
+      </c>
+      <c r="U3" t="s">
+        <v>100</v>
+      </c>
+      <c r="V3" t="s">
+        <v>101</v>
+      </c>
+      <c r="W3" t="s">
+        <v>102</v>
+      </c>
+      <c r="X3" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y3">
+        <v>756115</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L4" t="s">
+        <v>92</v>
+      </c>
+      <c r="M4" t="s">
+        <v>92</v>
+      </c>
+      <c r="N4" t="s">
+        <v>100</v>
+      </c>
+      <c r="O4" t="s">
+        <v>101</v>
+      </c>
+      <c r="P4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>102</v>
+      </c>
+      <c r="R4">
+        <v>756115</v>
+      </c>
+      <c r="S4" t="s">
+        <v>92</v>
+      </c>
+      <c r="T4" t="s">
+        <v>92</v>
+      </c>
+      <c r="U4" t="s">
+        <v>100</v>
+      </c>
+      <c r="V4" t="s">
+        <v>101</v>
+      </c>
+      <c r="W4" t="s">
+        <v>102</v>
+      </c>
+      <c r="X4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y4">
+        <v>756115</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" t="s">
+        <v>92</v>
+      </c>
+      <c r="M5" t="s">
+        <v>92</v>
+      </c>
+      <c r="N5" t="s">
+        <v>100</v>
+      </c>
+      <c r="O5" t="s">
+        <v>101</v>
+      </c>
+      <c r="P5" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>102</v>
+      </c>
+      <c r="R5">
+        <v>756115</v>
+      </c>
+      <c r="S5" t="s">
+        <v>92</v>
+      </c>
+      <c r="T5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U5" t="s">
+        <v>100</v>
+      </c>
+      <c r="V5" t="s">
+        <v>101</v>
+      </c>
+      <c r="W5" t="s">
+        <v>102</v>
+      </c>
+      <c r="X5" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y5">
+        <v>756115</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" t="s">
+        <v>88</v>
+      </c>
+      <c r="I6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" t="s">
+        <v>92</v>
+      </c>
+      <c r="M6" t="s">
+        <v>92</v>
+      </c>
+      <c r="N6" t="s">
+        <v>100</v>
+      </c>
+      <c r="O6" t="s">
+        <v>101</v>
+      </c>
+      <c r="P6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>102</v>
+      </c>
+      <c r="R6">
+        <v>756115</v>
+      </c>
+      <c r="S6" t="s">
+        <v>92</v>
+      </c>
+      <c r="T6" t="s">
+        <v>92</v>
+      </c>
+      <c r="U6" t="s">
+        <v>100</v>
+      </c>
+      <c r="V6" t="s">
+        <v>101</v>
+      </c>
+      <c r="W6" t="s">
+        <v>102</v>
+      </c>
+      <c r="X6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y6">
+        <v>756115</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" t="s">
+        <v>65</v>
+      </c>
+      <c r="K7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L7" t="s">
+        <v>92</v>
+      </c>
+      <c r="M7" t="s">
+        <v>92</v>
+      </c>
+      <c r="N7" t="s">
+        <v>100</v>
+      </c>
+      <c r="O7" t="s">
+        <v>101</v>
+      </c>
+      <c r="P7" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>102</v>
+      </c>
+      <c r="R7">
+        <v>756115</v>
+      </c>
+      <c r="S7" t="s">
+        <v>92</v>
+      </c>
+      <c r="T7" t="s">
+        <v>92</v>
+      </c>
+      <c r="U7" t="s">
+        <v>100</v>
+      </c>
+      <c r="V7" t="s">
+        <v>101</v>
+      </c>
+      <c r="W7" t="s">
+        <v>102</v>
+      </c>
+      <c r="X7" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y7">
+        <v>756115</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" t="s">
+        <v>92</v>
+      </c>
+      <c r="M8" t="s">
+        <v>92</v>
+      </c>
+      <c r="N8" t="s">
+        <v>100</v>
+      </c>
+      <c r="O8" t="s">
+        <v>101</v>
+      </c>
+      <c r="P8" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>102</v>
+      </c>
+      <c r="R8">
+        <v>756115</v>
+      </c>
+      <c r="S8" t="s">
+        <v>92</v>
+      </c>
+      <c r="T8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U8" t="s">
+        <v>100</v>
+      </c>
+      <c r="V8" t="s">
+        <v>101</v>
+      </c>
+      <c r="W8" t="s">
+        <v>102</v>
+      </c>
+      <c r="X8" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y8">
+        <v>756115</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M9" t="s">
+        <v>92</v>
+      </c>
+      <c r="N9" t="s">
+        <v>100</v>
+      </c>
+      <c r="O9" t="s">
+        <v>101</v>
+      </c>
+      <c r="P9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R9">
+        <v>756115</v>
+      </c>
+      <c r="S9" t="s">
+        <v>92</v>
+      </c>
+      <c r="T9" t="s">
+        <v>92</v>
+      </c>
+      <c r="U9" t="s">
+        <v>100</v>
+      </c>
+      <c r="V9" t="s">
+        <v>101</v>
+      </c>
+      <c r="W9" t="s">
+        <v>102</v>
+      </c>
+      <c r="X9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y9">
+        <v>756115</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" t="s">
+        <v>91</v>
+      </c>
+      <c r="I10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" t="s">
+        <v>62</v>
+      </c>
+      <c r="L10" t="s">
+        <v>92</v>
+      </c>
+      <c r="M10" t="s">
+        <v>92</v>
+      </c>
+      <c r="N10" t="s">
+        <v>100</v>
+      </c>
+      <c r="O10" t="s">
+        <v>101</v>
+      </c>
+      <c r="P10" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>102</v>
+      </c>
+      <c r="R10">
+        <v>756115</v>
+      </c>
+      <c r="S10" t="s">
+        <v>92</v>
+      </c>
+      <c r="T10" t="s">
+        <v>92</v>
+      </c>
+      <c r="U10" t="s">
+        <v>100</v>
+      </c>
+      <c r="V10" t="s">
+        <v>101</v>
+      </c>
+      <c r="W10" t="s">
+        <v>102</v>
+      </c>
+      <c r="X10" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y10">
+        <v>756115</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AA2" r:id="rId1"/>
+    <hyperlink ref="AB2" r:id="rId2"/>
+    <hyperlink ref="AC2" r:id="rId3"/>
+    <hyperlink ref="AA3" r:id="rId4"/>
+    <hyperlink ref="AA4" r:id="rId5"/>
+    <hyperlink ref="AA5" r:id="rId6"/>
+    <hyperlink ref="AA6" r:id="rId7"/>
+    <hyperlink ref="AA7" r:id="rId8"/>
+    <hyperlink ref="AA8" r:id="rId9"/>
+    <hyperlink ref="AA9" r:id="rId10"/>
+    <hyperlink ref="AA10" r:id="rId11"/>
+    <hyperlink ref="AB3" r:id="rId12"/>
+    <hyperlink ref="AC3" r:id="rId13"/>
+    <hyperlink ref="AB4" r:id="rId14"/>
+    <hyperlink ref="AC4" r:id="rId15"/>
+    <hyperlink ref="AB5" r:id="rId16"/>
+    <hyperlink ref="AC5" r:id="rId17"/>
+    <hyperlink ref="AB6" r:id="rId18"/>
+    <hyperlink ref="AC6" r:id="rId19"/>
+    <hyperlink ref="AB7" r:id="rId20"/>
+    <hyperlink ref="AC7" r:id="rId21"/>
+    <hyperlink ref="AB8" r:id="rId22"/>
+    <hyperlink ref="AC8" r:id="rId23"/>
+    <hyperlink ref="AB9" r:id="rId24"/>
+    <hyperlink ref="AC9" r:id="rId25"/>
+    <hyperlink ref="AB10" r:id="rId26"/>
+    <hyperlink ref="AC10" r:id="rId27"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -819,11 +1957,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="A1:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -861,14 +2012,8 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
       <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>14</v>
@@ -931,14 +2076,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>21</v>
+      <c r="A4" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -1204,6 +2349,7 @@
     <hyperlink ref="K9" r:id="rId25"/>
     <hyperlink ref="J10" r:id="rId26"/>
     <hyperlink ref="K10" r:id="rId27"/>
+    <hyperlink ref="A4" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>